<commit_message>
feat: add functional to project
</commit_message>
<xml_diff>
--- a/src/assets/excel/Svedeniya-ob-osushhestvlyaemyh-vidah-deyatelnosti.xlsx
+++ b/src/assets/excel/Svedeniya-ob-osushhestvlyaemyh-vidah-deyatelnosti.xlsx
@@ -1,15 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC5B10B-9FE1-44E5-9C1F-D24A3625D416}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -72,7 +71,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -237,73 +236,73 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -317,6 +316,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -365,7 +367,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -398,9 +400,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -433,6 +452,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -608,10 +644,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:I3"/>
     </sheetView>
   </sheetViews>
@@ -622,189 +658,189 @@
     <col min="6" max="6" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
     </row>
     <row r="3" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
     </row>
     <row r="5" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
     </row>
     <row r="6" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
     </row>
     <row r="7" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
     </row>
     <row r="8" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
     </row>
     <row r="9" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
+      <c r="A9" s="3">
         <v>6</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" ht="236.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="7" t="s">
+      <c r="B10" s="23"/>
+      <c r="C10" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="7" t="s">
+      <c r="D10" s="23"/>
+      <c r="E10" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="7" t="s">
+      <c r="F10" s="23"/>
+      <c r="G10" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="8"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="23"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="11"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="9"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="13"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="10"/>
       <c r="H12" s="15"/>
-      <c r="I12" s="14"/>
+      <c r="I12" s="11"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="17"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="13"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="19" t="s">
+      <c r="B14" s="18"/>
+      <c r="C14" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="20"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="18"/>
     </row>
     <row r="16" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" s="6" t="s">
@@ -817,27 +853,38 @@
       <c r="I17" s="6"/>
     </row>
     <row r="19" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="F20" s="5" t="s">
+      <c r="B20" s="7"/>
+      <c r="F20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
     <mergeCell ref="A16:I16"/>
     <mergeCell ref="D17:I17"/>
     <mergeCell ref="F20:I20"/>
@@ -850,43 +897,8 @@
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="G14:I14"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="A6:I6"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>